<commit_message>
more updates from milan
</commit_message>
<xml_diff>
--- a/BriefTasks 2013-09-08.xlsx
+++ b/BriefTasks 2013-09-08.xlsx
@@ -1525,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:XFD83"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="G133" sqref="A133:G133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3783,19 +3783,21 @@
       </c>
     </row>
     <row r="133" spans="1:8">
-      <c r="A133" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B133" s="22" t="s">
+      <c r="A133" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D133" s="3">
+      <c r="C133" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" s="15">
         <v>41511</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="E133" s="15"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="14" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>